<commit_message>
create file fn_acm, fn_springer
</commit_message>
<xml_diff>
--- a/ListadoArticulos.xlsx
+++ b/ListadoArticulos.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hogar\Desktop\11 - Herramientas\bot_busqueda\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3296AC42-12A9-44E3-94EE-062751440D5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,9 +24,71 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Links Articulos</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10937826</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/4053283</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10993799</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/8397647</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/6493605</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10270721</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10121659</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/9006200</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10158172</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/10423308</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/9842688</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/9006051</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s10586-024-04266-0</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/978-3-031-66329-1_38</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s00500-023-07989-1</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3416507.3423191</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3416507.3428118</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/10.1145/3416507.3423188</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +96,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,13 +128,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +416,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" xr:uid="{1B57B2B1-00AA-4F24-A5D3-661BC1A2FA22}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{66C9F03C-3257-4B97-ADE1-5F10AB91DE82}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{06F13A1B-A14C-431A-884A-06073BF41F92}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>